<commit_message>
updation to django files
</commit_message>
<xml_diff>
--- a/media/csv_files/detail2.xlsx
+++ b/media/csv_files/detail2.xlsx
@@ -1,15 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MainProject\Project\media\csv_files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB34956D-FFAD-41FF-9340-07210CA177CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="40" windowWidth="19100" windowHeight="7300"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -51,8 +55,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,13 +113,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -153,7 +165,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -187,6 +199,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -221,9 +234,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -396,20 +410,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="34.36328125" customWidth="1"/>
     <col min="4" max="4" width="24.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -423,7 +437,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -437,7 +451,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -451,7 +465,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -465,7 +479,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -481,34 +495,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3:C5" r:id="rId2" display="adrishyaabraham30@gmail.com"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C3:C5" r:id="rId2" display="adrishyaabraham30@gmail.com" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>